<commit_message>
solve parse xlsx issue
</commit_message>
<xml_diff>
--- a/cypress/fixtures/ordersData.excel.xlsx
+++ b/cypress/fixtures/ordersData.excel.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="28">
   <si>
     <t>isNewCustomer</t>
   </si>
@@ -88,6 +88,21 @@
   </si>
   <si>
     <t>03:45</t>
+  </si>
+  <si>
+    <t>Charl</t>
+  </si>
+  <si>
+    <t>1, 2</t>
+  </si>
+  <si>
+    <t>charl.basta@gmail.com</t>
+  </si>
+  <si>
+    <t>2023-05-17</t>
+  </si>
+  <si>
+    <t>05:45</t>
   </si>
 </sst>
 </file>
@@ -436,10 +451,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J3"/>
+  <dimension ref="A1:J4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+      <selection activeCell="J4" sqref="J4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -552,12 +567,45 @@
         <v>22</v>
       </c>
     </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="B4" s="1">
+        <v>118</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D4" s="1">
+        <v>4</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="H4" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="I4" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="J4" s="5" t="s">
+        <v>27</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="F2" r:id="rId1"/>
     <hyperlink ref="F3" r:id="rId2"/>
+    <hyperlink ref="F4" r:id="rId3"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId3"/>
+  <pageSetup orientation="portrait" r:id="rId4"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Add more test data
</commit_message>
<xml_diff>
--- a/cypress/fixtures/ordersData.excel.xlsx
+++ b/cypress/fixtures/ordersData.excel.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="31">
   <si>
     <t>isNewCustomer</t>
   </si>
@@ -103,6 +103,15 @@
   </si>
   <si>
     <t>05:45</t>
+  </si>
+  <si>
+    <t>Sami</t>
+  </si>
+  <si>
+    <t>1, 3</t>
+  </si>
+  <si>
+    <t>sami.basta@gmail.com</t>
   </si>
 </sst>
 </file>
@@ -451,10 +460,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J4"/>
+  <dimension ref="A1:J11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J4" sqref="J4"/>
+      <selection activeCell="H11" sqref="H11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -572,19 +581,19 @@
         <v>0</v>
       </c>
       <c r="B4" s="1">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>24</v>
+        <v>29</v>
       </c>
       <c r="D4" s="1">
         <v>4</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>23</v>
+        <v>28</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="G4" s="1" t="s">
         <v>5</v>
@@ -597,6 +606,230 @@
       </c>
       <c r="J4" s="5" t="s">
         <v>27</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="B5" s="1">
+        <v>229</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D5" s="1">
+        <v>4</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F5" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="G5" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="H5" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="I5" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="J5" s="5" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="B6" s="1">
+        <v>112</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D6" s="1">
+        <v>5</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F6" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="G6" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="H6" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="I6" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="J6" s="5" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="B7" s="1">
+        <v>110</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D7" s="1">
+        <v>4</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="F7" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="G7" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="H7" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="I7" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="J7" s="5" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="B8" s="1">
+        <v>227</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D8" s="1">
+        <v>4</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F8" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="G8" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="H8" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="I8" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="J8" s="5" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="B9" s="1">
+        <v>128</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D9" s="1">
+        <v>5</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F9" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="G9" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="H9" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="I9" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="J9" s="5" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A10" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="B10" s="1">
+        <v>145</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D10" s="1">
+        <v>4</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="F10" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="G10" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="H10" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="I10" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="J10" s="5" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A11" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="B11" s="1">
+        <v>235</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D11" s="1">
+        <v>4</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F11" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="G11" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="H11" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="I11" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="J11" s="5" t="s">
+        <v>21</v>
       </c>
     </row>
   </sheetData>
@@ -604,8 +837,15 @@
     <hyperlink ref="F2" r:id="rId1"/>
     <hyperlink ref="F3" r:id="rId2"/>
     <hyperlink ref="F4" r:id="rId3"/>
+    <hyperlink ref="F5" r:id="rId4"/>
+    <hyperlink ref="F6" r:id="rId5"/>
+    <hyperlink ref="F7" r:id="rId6"/>
+    <hyperlink ref="F8" r:id="rId7"/>
+    <hyperlink ref="F9" r:id="rId8"/>
+    <hyperlink ref="F10" r:id="rId9"/>
+    <hyperlink ref="F11" r:id="rId10"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId4"/>
+  <pageSetup orientation="portrait" r:id="rId11"/>
 </worksheet>
 </file>
</xml_diff>